<commit_message>
Changes to SPR excel file
</commit_message>
<xml_diff>
--- a/modules/SPR/Cases/SPR.xlsx
+++ b/modules/SPR/Cases/SPR.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaWork\Web\GitHub\NCNRS349\modules\Recruitment\Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaWork\Web\GitHub\NCNRS349\modules\SPR\Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15045" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15048" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>700-750</t>
   </si>
   <si>
-    <t>759-800</t>
-  </si>
-  <si>
     <t>800-850</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
       </rPr>
       <t>_i</t>
     </r>
+  </si>
+  <si>
+    <t>750-800</t>
   </si>
 </sst>
 </file>
@@ -342,6 +342,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -354,7 +355,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,43 +609,43 @@
                   <c:v>48.063560635555099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>349.6211263722721</c:v>
+                  <c:v>348.22543511022832</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1897.0816088401127</c:v>
+                  <c:v>2271.2190413624407</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6514.936999480039</c:v>
+                  <c:v>9189.8309431450416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9396.3067203087303</c:v>
+                  <c:v>15185.130765843995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8577.090840275152</c:v>
+                  <c:v>15319.013864765857</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7133.2648716409794</c:v>
+                  <c:v>14080.192688233808</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5852.7364121933988</c:v>
+                  <c:v>12767.582160471346</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4793.2051540944085</c:v>
+                  <c:v>11555.936898803664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3924.4985174798044</c:v>
+                  <c:v>10456.654571341804</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3213.1246968797727</c:v>
+                  <c:v>9461.6225899254714</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2630.6858942544413</c:v>
+                  <c:v>8561.2363101673927</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2153.82365289277</c:v>
+                  <c:v>7746.5277118648728</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1763.4016845519973</c:v>
+                  <c:v>7009.3482258527074</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,11 +660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142307120"/>
-        <c:axId val="142307512"/>
+        <c:axId val="263538288"/>
+        <c:axId val="263538672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142307120"/>
+        <c:axId val="263538288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -780,12 +780,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142307512"/>
+        <c:crossAx val="263538672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142307512"/>
+        <c:axId val="263538672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -900,7 +900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142307120"/>
+        <c:crossAx val="263538288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1110,11 +1110,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142308296"/>
-        <c:axId val="142308688"/>
+        <c:axId val="263670240"/>
+        <c:axId val="263670624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142308296"/>
+        <c:axId val="263670240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -1230,12 +1230,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142308688"/>
+        <c:crossAx val="263670624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142308688"/>
+        <c:axId val="263670624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1360,7 +1360,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142308296"/>
+        <c:crossAx val="263670240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1567,11 +1567,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142309472"/>
-        <c:axId val="142309864"/>
+        <c:axId val="264002040"/>
+        <c:axId val="264010616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142309472"/>
+        <c:axId val="264002040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -1687,12 +1687,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142309864"/>
+        <c:crossAx val="264010616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142309864"/>
+        <c:axId val="264010616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1807,7 +1807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142309472"/>
+        <c:crossAx val="264002040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -2096,43 +2096,43 @@
                   <c:v>0.77880078307140488</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60653065971263342</c:v>
+                  <c:v>0.60410938285586468</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38674102345450123</c:v>
+                  <c:v>0.46301306831122807</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24659696394160652</c:v>
+                  <c:v>0.34784440891708746</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15723716631362766</c:v>
+                  <c:v>0.25410695955280033</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10025884372280378</c:v>
+                  <c:v>0.17906614791149325</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3927861206707598E-2</c:v>
+                  <c:v>0.12618578170503877</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0762203978366232E-2</c:v>
+                  <c:v>8.8921617459386357E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5991128778755358E-2</c:v>
+                  <c:v>6.2662004742153166E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6572675401761258E-2</c:v>
+                  <c:v>4.4157168419692874E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0567204383852662E-2</c:v>
+                  <c:v>3.1117030661060873E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.7379469990854731E-3</c:v>
+                  <c:v>2.192780089426162E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.296304690752345E-3</c:v>
+                  <c:v>1.5452260123909517E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7394448187683723E-3</c:v>
+                  <c:v>1.0889023668554447E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2147,11 +2147,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142310648"/>
-        <c:axId val="142311040"/>
+        <c:axId val="262541496"/>
+        <c:axId val="262541888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142310648"/>
+        <c:axId val="262541496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -2267,12 +2267,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142311040"/>
+        <c:crossAx val="262541888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142311040"/>
+        <c:axId val="262541888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2397,7 +2397,455 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142310648"/>
+        <c:crossAx val="262541496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>slctvty</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="264193640"/>
+        <c:axId val="264194032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="264193640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="900"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Length (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="264194032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="264194032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Selectivity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="264193640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2606,6 +3054,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4155,6 +4643,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4798,6 +5802,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>572214</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>70919</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5066,24 +6102,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="7.796875" customWidth="1"/>
-    <col min="4" max="4" width="6.59765625" customWidth="1"/>
-    <col min="5" max="5" width="5.796875" customWidth="1"/>
-    <col min="6" max="6" width="6.69921875" customWidth="1"/>
-    <col min="7" max="7" width="6.296875" customWidth="1"/>
-    <col min="9" max="9" width="5.5" customWidth="1"/>
-    <col min="10" max="10" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.8984375" customWidth="1"/>
-    <col min="12" max="12" width="6.296875" customWidth="1"/>
-    <col min="13" max="13" width="9.296875" customWidth="1"/>
-    <col min="14" max="14" width="4.59765625" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
@@ -5117,42 +6154,42 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="27"/>
+      <c r="A3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="28"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="18">
         <v>0.25</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="26" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>2</v>
@@ -5182,7 +6219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -5193,7 +6230,7 @@
         <f>EXP($C$1+$C$2*B5)</f>
         <v>24959.255641914595</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="25">
         <f>1/(1+EXP($D$1-$D$2*B5))</f>
         <v>2.4726231566347743E-3</v>
       </c>
@@ -5233,7 +6270,7 @@
         <v>48.063560635555099</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -5244,7 +6281,7 @@
         <f t="shared" ref="C6:C18" si="2">EXP($C$1+$C$2*B6)</f>
         <v>32048.31862582525</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="25">
         <f t="shared" ref="D6:D18" si="3">1/(1+EXP($D$1-$D$2*B6))</f>
         <v>1.7986209962091559E-2</v>
       </c>
@@ -5266,25 +6303,25 @@
       </c>
       <c r="I6" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="J6" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K6" s="10">
         <f t="shared" ref="K6:K18" si="6">EXP(-(E6+I6*J6))</f>
-        <v>0.77880078307140488</v>
+        <v>0.77569180204647603</v>
       </c>
       <c r="L6" s="10">
         <f>L5*K6</f>
-        <v>0.60653065971263342</v>
+        <v>0.60410938285586468</v>
       </c>
       <c r="M6" s="11">
         <f t="shared" ref="M6:M18" si="7">C6*D6*L6</f>
-        <v>349.6211263722721</v>
+        <v>348.22543511022832</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -5295,7 +6332,7 @@
         <f t="shared" si="2"/>
         <v>41150.855677666768</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="25">
         <f t="shared" si="3"/>
         <v>0.11920292202211755</v>
       </c>
@@ -5317,25 +6354,25 @@
       </c>
       <c r="I7" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="J7" s="22">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="K7" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.76643912750101917</v>
       </c>
       <c r="L7" s="10">
         <f t="shared" ref="L7:L18" si="9">L6*K7</f>
-        <v>0.38674102345450123</v>
+        <v>0.46301306831122807</v>
       </c>
       <c r="M7" s="11">
         <f t="shared" si="7"/>
-        <v>1897.0816088401127</v>
+        <v>2271.2190413624407</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -5346,7 +6383,7 @@
         <f t="shared" si="2"/>
         <v>52838.744608573186</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="25">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -5368,25 +6405,25 @@
       </c>
       <c r="I8" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.06</v>
       </c>
       <c r="J8" s="22">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="K8" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.75126261594688604</v>
       </c>
       <c r="L8" s="10">
         <f t="shared" si="9"/>
-        <v>0.24659696394160652</v>
+        <v>0.34784440891708746</v>
       </c>
       <c r="M8" s="11">
         <f t="shared" si="7"/>
-        <v>6514.936999480039</v>
+        <v>9189.8309431450416</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -5397,7 +6434,7 @@
         <f t="shared" si="2"/>
         <v>67846.29106328034</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="25">
         <f t="shared" si="3"/>
         <v>0.88079707797788231</v>
       </c>
@@ -5419,25 +6456,25 @@
       </c>
       <c r="I9" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="J9" s="22">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K9" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.73051902815942493</v>
       </c>
       <c r="L9" s="10">
         <f t="shared" si="9"/>
-        <v>0.15723716631362766</v>
+        <v>0.25410695955280033</v>
       </c>
       <c r="M9" s="11">
         <f t="shared" si="7"/>
-        <v>9396.3067203087303</v>
+        <v>15185.130765843995</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -5448,7 +6485,7 @@
         <f t="shared" si="2"/>
         <v>87116.362153246329</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="25">
         <f t="shared" si="3"/>
         <v>0.98201379003790845</v>
       </c>
@@ -5470,25 +6507,25 @@
       </c>
       <c r="I10" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J10" s="22">
         <v>1</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L10" s="10">
         <f t="shared" si="9"/>
-        <v>0.10025884372280378</v>
+        <v>0.17906614791149325</v>
       </c>
       <c r="M10" s="11">
         <f t="shared" si="7"/>
-        <v>8577.090840275152</v>
+        <v>15319.013864765857</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -5499,7 +6536,7 @@
         <f t="shared" si="2"/>
         <v>111859.62321414231</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="25">
         <f t="shared" si="3"/>
         <v>0.99752737684336534</v>
       </c>
@@ -5521,25 +6558,25 @@
       </c>
       <c r="I11" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J11" s="22">
         <v>1</v>
       </c>
       <c r="K11" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L11" s="10">
         <f t="shared" si="9"/>
-        <v>6.3927861206707598E-2</v>
+        <v>0.12618578170503877</v>
       </c>
       <c r="M11" s="11">
         <f t="shared" si="7"/>
-        <v>7133.2648716409794</v>
+        <v>14080.192688233808</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -5550,7 +6587,7 @@
         <f t="shared" si="2"/>
         <v>143630.59930807285</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="25">
         <f t="shared" si="3"/>
         <v>0.99966464986953363</v>
       </c>
@@ -5572,25 +6609,25 @@
       </c>
       <c r="I12" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J12" s="22">
         <v>1</v>
       </c>
       <c r="K12" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L12" s="10">
         <f t="shared" si="9"/>
-        <v>4.0762203978366232E-2</v>
+        <v>8.8921617459386357E-2</v>
       </c>
       <c r="M12" s="11">
         <f t="shared" si="7"/>
-        <v>5852.7364121933988</v>
+        <v>12767.582160471346</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -5601,7 +6638,7 @@
         <f t="shared" si="2"/>
         <v>184425.34012565826</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="25">
         <f t="shared" si="3"/>
         <v>0.99995460213129761</v>
       </c>
@@ -5623,25 +6660,25 @@
       </c>
       <c r="I13" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J13" s="22">
         <v>1</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="9"/>
-        <v>2.5991128778755358E-2</v>
+        <v>6.2662004742153166E-2</v>
       </c>
       <c r="M13" s="11">
         <f t="shared" si="7"/>
-        <v>4793.2051540944085</v>
+        <v>11555.936898803664</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -5652,7 +6689,7 @@
         <f t="shared" si="2"/>
         <v>236806.8242026268</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="25">
         <f t="shared" si="3"/>
         <v>0.99999385582539779</v>
       </c>
@@ -5674,25 +6711,25 @@
       </c>
       <c r="I14" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J14" s="22">
         <v>1</v>
       </c>
       <c r="K14" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L14" s="10">
         <f t="shared" si="9"/>
-        <v>1.6572675401761258E-2</v>
+        <v>4.4157168419692874E-2</v>
       </c>
       <c r="M14" s="11">
         <f t="shared" si="7"/>
-        <v>3924.4985174798044</v>
+        <v>10456.654571341804</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -5703,7 +6740,7 @@
         <f t="shared" si="2"/>
         <v>304065.98112127866</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="25">
         <f t="shared" si="3"/>
         <v>0.99999916847197223</v>
       </c>
@@ -5725,27 +6762,27 @@
       </c>
       <c r="I15" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J15" s="22">
         <v>1</v>
       </c>
       <c r="K15" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L15" s="10">
         <f t="shared" si="9"/>
-        <v>1.0567204383852662E-2</v>
+        <v>3.1117030661060873E-2</v>
       </c>
       <c r="M15" s="11">
         <f t="shared" si="7"/>
-        <v>3213.1246968797727</v>
+        <v>9461.6225899254714</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1">
         <v>775</v>
@@ -5754,7 +6791,7 @@
         <f t="shared" si="2"/>
         <v>390428.44810981676</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="25">
         <f t="shared" si="3"/>
         <v>0.99999988746483792</v>
       </c>
@@ -5776,27 +6813,27 @@
       </c>
       <c r="I16" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J16" s="22">
         <v>1</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L16" s="10">
         <f t="shared" si="9"/>
-        <v>6.7379469990854731E-3</v>
+        <v>2.192780089426162E-2</v>
       </c>
       <c r="M16" s="11">
         <f t="shared" si="7"/>
-        <v>2630.6858942544413</v>
+        <v>8561.2363101673927</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="13.95" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>825</v>
@@ -5805,7 +6842,7 @@
         <f t="shared" si="2"/>
         <v>501320.05077095568</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="25">
         <f t="shared" si="3"/>
         <v>0.9999999847700205</v>
       </c>
@@ -5827,27 +6864,27 @@
       </c>
       <c r="I17" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J17" s="22">
         <v>1</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L17" s="10">
         <f t="shared" si="9"/>
-        <v>4.296304690752345E-3</v>
+        <v>1.5452260123909517E-2</v>
       </c>
       <c r="M17" s="11">
         <f t="shared" si="7"/>
-        <v>2153.82365289277</v>
+        <v>7746.5277118648728</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
         <v>875</v>
@@ -5856,7 +6893,7 @@
         <f t="shared" si="2"/>
         <v>643707.68708509614</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="25">
         <f t="shared" si="3"/>
         <v>0.99999999793884631</v>
       </c>
@@ -5878,25 +6915,25 @@
       </c>
       <c r="I18" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J18" s="23">
         <v>1</v>
       </c>
       <c r="K18" s="10">
         <f t="shared" si="6"/>
-        <v>0.63762815162177333</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="L18" s="10">
         <f t="shared" si="9"/>
-        <v>2.7394448187683723E-3</v>
+        <v>1.0889023668554447E-2</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" si="7"/>
-        <v>1763.4016845519973</v>
+        <v>7009.3482258527074</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="13.95" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
         <v>5</v>
       </c>
@@ -5909,16 +6946,16 @@
       </c>
       <c r="M19">
         <f>SUM(M5:M18)</f>
-        <v>58247.841739899435</v>
+        <v>124000.58476752418</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="13.95" x14ac:dyDescent="0.3">
       <c r="L20" s="13" t="s">
         <v>6</v>
       </c>
       <c r="M20" s="13">
         <f>M19/H19</f>
-        <v>0.28539645391429608</v>
+        <v>0.6075646087279658</v>
       </c>
       <c r="N20" s="14" t="str">
         <f>IF(M20&lt;$L$1,"YES","no")</f>
@@ -5945,14 +6982,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">

</xml_diff>